<commit_message>
REgenerate instance 00 and 01
</commit_message>
<xml_diff>
--- a/Instances/00_Binomial.xlsx
+++ b/Instances/00_Binomial.xlsx
@@ -808,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
         <v>0.026</v>
@@ -1170,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>140</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1178,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>70</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1186,7 +1186,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>35</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1202,7 +1202,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>70</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1246,7 +1246,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -1292,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1338,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify create script Regenerate instances
</commit_message>
<xml_diff>
--- a/Instances/00_Binomial.xlsx
+++ b/Instances/00_Binomial.xlsx
@@ -698,7 +698,7 @@
         <v>0.026</v>
       </c>
       <c r="E2" t="n">
-        <v>0.091</v>
+        <v>0.0182</v>
       </c>
       <c r="F2" t="n">
         <v>0.26</v>
@@ -721,13 +721,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D3" t="n">
         <v>0.0048</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0168</v>
+        <v>0.003360000000000001</v>
       </c>
       <c r="F3" t="n">
         <v>0.048</v>
@@ -750,13 +750,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D4" t="n">
         <v>0.002</v>
       </c>
       <c r="E4" t="n">
-        <v>0.007</v>
+        <v>0.0014</v>
       </c>
       <c r="F4" t="n">
         <v>0.02</v>
@@ -779,13 +779,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
         <v>0.0036</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0126</v>
+        <v>0.002520000000000001</v>
       </c>
       <c r="F5" t="n">
         <v>0.036</v>
@@ -808,13 +808,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6" t="n">
         <v>0.026</v>
       </c>
       <c r="E6" t="n">
-        <v>0.091</v>
+        <v>0.0182</v>
       </c>
       <c r="F6" t="n">
         <v>0.26</v>
@@ -1178,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>175</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1194,7 +1194,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1202,7 +1202,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>175</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -1315,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1338,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>